<commit_message>
🔄 Actualización automática del mapa (mapa_interactivo_INCO.html)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1334,7 +1334,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-173</t>
+          <t>-174</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1344,7 +1344,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>PACHECO DE MELO J A /ALT/ 2300</t>
+          <t>QUINTANA PTE M ,AV. /ALT/ 591</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1354,7 +1354,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>799539473</t>
+          <t>799539617</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1369,7 +1369,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal con inclinación en superficie y un poco de corrosión en base sin riesgo caída por lo cual dicho poste está obstruyendo entrada al colegio a pocos metros de dicha entrada </t>
+          <t>P. Quintana 591 ¿ Cambiar C168 ¿ NEW.</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1379,10 +1379,10 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
-        <v>-58.397535</v>
+        <v>-58.390647</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.588772</v>
+        <v>-34.587717</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1398,7 +1398,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>-174</t>
+          <t>-186</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1408,17 +1408,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>QUINTANA PTE M ,AV. /ALT/ 591</t>
+          <t>GAONA ,AV. /ALT/ 3757</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>799539617</t>
+          <t>799539793</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1433,7 +1433,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>P. Quintana 591 ¿ Cambiar C168 ¿ NEW.</t>
+          <t>Gaona 3757 columna podrida</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1443,26 +1443,26 @@
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
-        <v>-58.390647</v>
+        <v>-58.477557</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.587717</v>
+        <v>-34.622154</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>-186</t>
+          <t>-187</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1472,17 +1472,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>GAONA ,AV. /ALT/ 3757</t>
+          <t>ZAPIOLA /ALT/ 703</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>799539793</t>
+          <t>799539824</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1497,36 +1497,36 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Gaona 3757 columna podrida</t>
+          <t>- alt correcta 704</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="n">
-        <v>-58.477557</v>
+        <v>-58.448465</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.622154</v>
+        <v>-34.575944</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>-187</t>
+          <t>-195</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1536,17 +1536,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ZAPIOLA /ALT/ 703</t>
+          <t>ARIAS /ALT/ 3701</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>799539824</t>
+          <t>799540358</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1561,36 +1561,36 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>- alt correcta 704</t>
+          <t>Retirar poste y colocar columna a plomo, traspasar linda de poste a columna. Arias esquina Melian casa 166. Solicita Horacio Alvarez.</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
-        <v>-58.448465</v>
+        <v>-58.485782</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.575944</v>
+        <v>-34.547305</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>-195</t>
+          <t>-196</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1600,7 +1600,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ARIAS /ALT/ 3701</t>
+          <t>CORREA CIRILO /ALT/ 3868</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1610,7 +1610,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>799540358</t>
+          <t>799540449</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1625,20 +1625,20 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Retirar poste y colocar columna a plomo, traspasar linda de poste a columna. Arias esquina Melian casa 166. Solicita Horacio Alvarez.</t>
+          <t>Columna picada en base, informa el GCBA</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="n">
-        <v>-58.485782</v>
+        <v>-58.486971</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.547305</v>
+        <v>-34.550135</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>-196</t>
+          <t>-197</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1664,7 +1664,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>CORREA CIRILO /ALT/ 3868</t>
+          <t>LOPEZ BUCHARDO C /ALT/ 5606</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1674,7 +1674,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>799540449</t>
+          <t>799540455</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1687,26 +1687,22 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Columna picada en base, informa el GCBA</t>
-        </is>
-      </c>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
-        <v>-58.486971</v>
+        <v>-58.500508</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.550135</v>
+        <v>-34.563097</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1718,7 +1714,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-197</t>
+          <t>-198</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1728,7 +1724,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>LOPEZ BUCHARDO C /ALT/ 5606</t>
+          <t>PEREZ ROQUE /ALT/ 4548</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1738,7 +1734,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>799540455</t>
+          <t>799540475</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1759,14 +1755,14 @@
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
-        <v>-58.500508</v>
+        <v>-58.484555</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.563097</v>
+        <v>-34.547242</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -1778,7 +1774,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-198</t>
+          <t>-199</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1788,7 +1784,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>PEREZ ROQUE /ALT/ 4548</t>
+          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4661</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1798,7 +1794,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>799540475</t>
+          <t>799540477</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1811,7 +1807,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Poste quebrado</t>
+        </is>
+      </c>
       <c r="I22" t="n">
         <v>0</v>
       </c>
@@ -1819,10 +1819,10 @@
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="n">
-        <v>-58.484555</v>
+        <v>-58.493565</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.547242</v>
+        <v>-34.554439</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -1838,7 +1838,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-199</t>
+          <t>-200</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1848,7 +1848,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4661</t>
+          <t>BALBIN RICARDO ,AV. /ALT/ 3528</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1858,7 +1858,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>799540477</t>
+          <t>799540489</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1871,11 +1871,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Poste quebrado</t>
-        </is>
-      </c>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="n">
         <v>0</v>
       </c>
@@ -1883,10 +1879,10 @@
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="n">
-        <v>-58.493565</v>
+        <v>-58.480334</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.554439</v>
+        <v>-34.556445</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -1902,7 +1898,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-200</t>
+          <t>-209</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1912,17 +1908,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>BALBIN RICARDO ,AV. /ALT/ 3528</t>
+          <t>PICO /ALT/ 1654</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>799540489</t>
+          <t>799540564</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1935,7 +1931,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr"/>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Pico 1654 / 1650 cambiar columna 114 efectuar transferencias contactar a Telecentro para transferir el Nodo</t>
+        </is>
+      </c>
       <c r="I24" t="n">
         <v>0</v>
       </c>
@@ -1943,10 +1943,10 @@
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="n">
-        <v>-58.480334</v>
+        <v>-58.466988</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.556445</v>
+        <v>-34.537094</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -1962,27 +1962,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-209</t>
+          <t>-211</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>PICO /ALT/ 1654</t>
+          <t>BOYACA ,AV. /ALT/ 2030</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>799540564</t>
+          <t>799488822</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1995,11 +1995,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>Pico 1654 / 1650 cambiar columna 114 efectuar transferencias contactar a Telecentro para transferir el Nodo</t>
-        </is>
-      </c>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
         <v>0</v>
       </c>
@@ -2007,14 +2003,14 @@
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="n">
-        <v>-58.466988</v>
+        <v>-58.471173</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.537094</v>
+        <v>-34.60704</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2026,27 +2022,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-211</t>
+          <t>-218</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>9/26/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>BOYACA ,AV. /ALT/ 2030</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>799488822</t>
+          <t>797118027</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2059,7 +2055,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
       <c r="I26" t="n">
         <v>0</v>
       </c>
@@ -2067,46 +2067,46 @@
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="n">
-        <v>-58.471173</v>
+        <v>-58.395465</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.60704</v>
+        <v>-34.622784</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-218</t>
+          <t>-225</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>9/26/2024</t>
+          <t>11/19/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>SCALABRINI ORTIZ R ,AV. /ALT/ 213</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>797118027</t>
+          <t>800498182</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Colocar columna medianera 213/15</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2131,46 +2131,46 @@
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="n">
-        <v>-58.395465</v>
+        <v>-58.439714</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.622784</v>
+        <v>-34.600565</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-225</t>
+          <t>-235</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>11/19/2024</t>
+          <t>12/16/2024</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ R ,AV. /ALT/ 213</t>
+          <t>GUARDIA VIEJA /ALT/ 3457</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>800498182</t>
+          <t>801645807</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2183,11 +2183,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Colocar columna medianera 213/15</t>
-        </is>
-      </c>
+      <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
         <v>0</v>
       </c>
@@ -2195,26 +2191,26 @@
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="n">
-        <v>-58.439714</v>
+        <v>-58.413407</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.600565</v>
+        <v>-34.602292</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-235</t>
+          <t>-241</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2224,17 +2220,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>GUARDIA VIEJA /ALT/ 3457</t>
+          <t>CUENCA /ALT/ 116</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>801645807</t>
+          <t>801679775</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2247,7 +2243,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Podrida en base sin riego </t>
+        </is>
+      </c>
       <c r="I29" t="n">
         <v>0</v>
       </c>
@@ -2255,46 +2255,46 @@
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="n">
-        <v>-58.413407</v>
+        <v>-58.474354</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.602292</v>
+        <v>-34.629997</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-241</t>
+          <t>-247</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>12/16/2024</t>
+          <t>12/26/2024</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>CUENCA /ALT/ 116</t>
+          <t>CONCORDIA /ALT/ 925</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>801679775</t>
+          <t>802055232</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2309,20 +2309,32 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en base sin riego </t>
+          <t>Pasante con priroidad</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
-      </c>
-      <c r="J30" t="inlineStr"/>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M30" t="n">
-        <v>-58.474354</v>
+        <v>-58.479695</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.629997</v>
+        <v>-34.622867</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2338,27 +2350,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-247</t>
+          <t>-255</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>12/26/2024</t>
+          <t>1/8/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>CONCORDIA /ALT/ 925</t>
+          <t>GURRUCHAGA /ALT/ 408</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>802055232</t>
+          <t>802393948</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2371,11 +2383,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Pasante con priroidad</t>
-        </is>
-      </c>
+      <c r="H31" t="inlineStr"/>
       <c r="I31" t="n">
         <v>1</v>
       </c>
@@ -2386,7 +2394,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2395,14 +2403,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.479695</v>
+        <v>-58.442667</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.622867</v>
+        <v>-34.597977</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2414,27 +2422,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-255</t>
+          <t>-258</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1/8/2025</t>
+          <t>1/14/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>GURRUCHAGA /ALT/ 408</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 1465</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>802393948</t>
+          <t>802608477</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2447,7 +2455,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr"/>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I32" t="n">
         <v>1</v>
       </c>
@@ -2458,7 +2470,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2467,14 +2479,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.442667</v>
+        <v>-58.452317</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.597977</v>
+        <v>-34.567846</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2486,27 +2498,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-258</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>1/14/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 1465</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>802608477</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2521,7 +2533,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2543,14 +2555,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.452317</v>
+        <v>-58.480871</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.567846</v>
+        <v>-34.616598</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2562,27 +2574,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2597,7 +2609,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2619,46 +2631,46 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.480871</v>
+        <v>-58.407076</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.616598</v>
+        <v>-34.616016</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2673,7 +2685,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -2695,93 +2707,17 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.407076</v>
+        <v>-58.372751</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.616016</v>
+        <v>-34.631917</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>6180</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>5/4/2025</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>AZARA 15</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>805655333</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I36" t="n">
-        <v>1</v>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M36" t="n">
-        <v>-58.372751</v>
-      </c>
-      <c r="N36" t="n">
-        <v>-34.631917</v>
-      </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P36" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>